<commit_message>
Save results done. Bug in the conditional: Heavy-Old-Female shouldnt be 100
</commit_message>
<xml_diff>
--- a/SampleData.xlsx
+++ b/SampleData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
   <si>
     <t>Weight</t>
   </si>
@@ -63,7 +63,13 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>Sheet2:C3</t>
+    <t>Results:A1</t>
+  </si>
+  <si>
+    <t>Destination File</t>
+  </si>
+  <si>
+    <t>Results.xlsx</t>
   </si>
   <si>
     <t>Rules - Weight</t>
@@ -130,7 +136,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -149,12 +155,6 @@
     </font>
     <font>
       <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Ubuntu"/>
-      <charset val="1"/>
       <family val="0"/>
       <sz val="10"/>
     </font>
@@ -206,7 +206,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -315,10 +315,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E19"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="E13" activeCellId="0" pane="topLeft" sqref="E13"/>
+      <selection activeCell="C8" activeCellId="0" pane="topLeft" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -326,7 +326,7 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="18.8010204081633"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.95408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.08163265306122"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -368,16 +368,16 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="B9" s="0" t="s">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="8">
+      <c r="B8" s="0" t="s">
         <v>16</v>
       </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="C10" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="0" t="s">
+      <c r="B10" s="0" t="s">
         <v>18</v>
       </c>
     </row>
@@ -398,15 +398,15 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="D13" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="C14" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="B14" s="0" t="s">
         <v>25</v>
       </c>
     </row>
@@ -418,7 +418,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="16">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
         <v>28</v>
       </c>
@@ -427,24 +427,32 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="17">
-      <c r="B17" s="0" t="s">
+      <c r="C17" s="0" t="s">
         <v>30</v>
       </c>
+      <c r="D17" s="0" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="18">
-      <c r="C18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="B18" s="0" t="s">
         <v>32</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+      <c r="C20" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>